<commit_message>
Scan full file, ignore None
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>your</t>
   </si>
@@ -52,6 +52,300 @@
   </si>
   <si>
     <t>Jesse</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>it's</t>
+  </si>
+  <si>
+    <t>you're</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>already</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>another</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>believes</t>
+  </si>
+  <si>
+    <t>better</t>
+  </si>
+  <si>
+    <t>bringing</t>
+  </si>
+  <si>
+    <t>but</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>did</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>doesn't</t>
+  </si>
+  <si>
+    <t>doing</t>
+  </si>
+  <si>
+    <t>don't</t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>everything</t>
+  </si>
+  <si>
+    <t>felt</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>give</t>
+  </si>
+  <si>
+    <t>goddamn</t>
+  </si>
+  <si>
+    <t>going</t>
+  </si>
+  <si>
+    <t>got</t>
+  </si>
+  <si>
+    <t>handle</t>
+  </si>
+  <si>
+    <t>hands</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>have</t>
+  </si>
+  <si>
+    <t>he</t>
+  </si>
+  <si>
+    <t>hear</t>
+  </si>
+  <si>
+    <t>her</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>i'm</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>informant</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>just</t>
+  </si>
+  <si>
+    <t>kill</t>
+  </si>
+  <si>
+    <t>know</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>little</t>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t>matter</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>morpheus</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>need</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>relieve</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>sent</t>
+  </si>
+  <si>
+    <t>she</t>
+  </si>
+  <si>
+    <t>specific</t>
+  </si>
+  <si>
+    <t>sure</t>
+  </si>
+  <si>
+    <t>taking</t>
+  </si>
+  <si>
+    <t>that</t>
+  </si>
+  <si>
+    <t>that's</t>
+  </si>
+  <si>
+    <t>their</t>
+  </si>
+  <si>
+    <t>there</t>
+  </si>
+  <si>
+    <t>there's</t>
+  </si>
+  <si>
+    <t>they</t>
+  </si>
+  <si>
+    <t>they're</t>
+  </si>
+  <si>
+    <t>think</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>trinity</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>was</t>
+  </si>
+  <si>
+    <t>watching</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>we'll</t>
+  </si>
+  <si>
+    <t>we're</t>
+  </si>
+  <si>
+    <t>wells</t>
+  </si>
+  <si>
+    <t>were</t>
+  </si>
+  <si>
+    <t>what</t>
+  </si>
+  <si>
+    <t>white</t>
   </si>
 </sst>
 </file>
@@ -370,67 +664,561 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>